<commit_message>
.S03P31B104-15 .S03P31B104-17 | ADD | 영상, 자막 추가
</commit_message>
<xml_diff>
--- a/data/Subs_SK_1027.xlsx
+++ b/data/Subs_SK_1027.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ssafy\workspace\PJ3\s03p31b104\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,11 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$44</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="119">
   <si>
     <t>제목</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -49,10 +53,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>슈퍼주니어, 동방신기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SM타운 아날로그 트립여행 EP2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -150,28 +150,12 @@
     <t>https://www.youtube.com/watch?v=tP7S34Cgnr0&amp;list=PLA91TLEzZINv_5ZfZVFrEnyjIn5w1-zMq&amp;index=13</t>
   </si>
   <si>
-    <t>방탄소년단</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>레드벨벳</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이린, 슬기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=z3_M-FUVaS8&amp;list=WL&amp;index=6</t>
   </si>
   <si>
     <t>런닝맨왕코몰이2</t>
   </si>
   <si>
-    <t>블랙핑크</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=wcA2x_XumuM</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -197,10 +181,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>여자친구</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=nAjS-qnItF0&amp;list=RDCMUCUyfkq9e9ZfPzxOW5WQ9rzQ&amp;index=8</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -213,10 +193,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>세븐틴</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=yHXa9Sz3_6Y&amp;list=RDCMUCUyfkq9e9ZfPzxOW5WQ9rzQ&amp;index=18</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -237,10 +213,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>오마이걸</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>[문명특급 EP.132] 외출복 입고 침대 눕기 가능 vs 불가능, 여자친구랑 재재랑 취향 딱 나뉨 소름;;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -257,14 +229,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>티아라</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지연</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=hSoZgSwM394&amp;list=RDCMUCUyfkq9e9ZfPzxOW5WQ9rzQ&amp;index=27</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -285,14 +249,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>카라</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>니콜</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=gQ0PVNo_hu8&amp;list=RDCMUCUyfkq9e9ZfPzxOW5WQ9rzQ&amp;index=27</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -301,10 +257,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>효민</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=iUm9nERTP7Q&amp;list=RDCMUCUyfkq9e9ZfPzxOW5WQ9rzQ&amp;index=27</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -329,10 +281,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>선미</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=8jpJgAiHdJE&amp;list=RDCMUCUyfkq9e9ZfPzxOW5WQ9rzQ&amp;index=27</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -341,10 +289,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>에이프릴</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=xJYBANCAfhk&amp;list=RDCMUCUyfkq9e9ZfPzxOW5WQ9rzQ&amp;index=27</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -357,14 +301,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>[문명특급 EP.115] 정신머리(?) 없는 재재 팬, 몬스타엑스(monstaX )의 역팬싸 현장;; 정말 FANTASIA(판타지아)☆</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>몬스타엑스</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>[문명특급 EP.114] 요즘 아이돌(투모로우바이투게더) 스토리텔링 수준ㄷㄷ;; CAN'T YOU SEE ME?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -397,10 +333,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>우주소녀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=AAb4Sh0Rc9Y&amp;list=RDCMUCUyfkq9e9ZfPzxOW5WQ9rzQ&amp;index=27</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -469,11 +401,78 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Super Junior</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>희철</t>
+    <t>BTS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RED VELVET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BLACK PINK</t>
+  </si>
+  <si>
+    <t>MONSTA X</t>
+  </si>
+  <si>
+    <t>WJSN</t>
+  </si>
+  <si>
+    <t>SUPER JUNIOR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUPER JUNIOR, TVXQ</t>
+  </si>
+  <si>
+    <t>GFRIEND</t>
+  </si>
+  <si>
+    <t>SEVENTEEN</t>
+  </si>
+  <si>
+    <t>OHMYGIRL</t>
+  </si>
+  <si>
+    <t>T-ARA</t>
+  </si>
+  <si>
+    <t>Jiyeon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hyomin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RED VELVEL</t>
+  </si>
+  <si>
+    <t>Irene, Seulgi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KARA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nicole</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heechul</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>APRIL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUNMI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[문명특급 EP.115] 정신머리(?) 없는 재재 팬, 몬스타엑스(monstaX )의 역팬싸 현장;; 정말 FANTASIA(판타지아)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -866,7 +865,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H4" sqref="H4"/>
+      <selection pane="topRight" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -897,7 +896,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -905,488 +904,489 @@
     </row>
     <row r="3" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="87" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B44"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>